<commit_message>
adicionado roc curve, decision tree e random forest, experimentos estratificados
</commit_message>
<xml_diff>
--- a/DAGroup/notebooks/generated_data/pns_data_models/importances.xlsx
+++ b/DAGroup/notebooks/generated_data/pns_data_models/importances.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,91 @@
           <t>log_best_grid</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>log_class_renda_baixa</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>log_class_renda_alta</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>log_class_sexo_mulher</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>log_class_sexo_homem</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>log_class_idade_less40</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>log_class_idade_more40</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>log_class_idade1</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>log_class_idade2</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>log_class_idade3</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>log_class_idade4</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>log_class_r_norte</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>log_class_r_nordeste</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>log_class_r_sudeste</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>log_class_r_sul</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>log_class_r_centro_oeste</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>dt_exp</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>rf_exp</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -487,29 +572,76 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.0740584482662671</v>
+        <v>0.08841029047095439</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.3561407160458364</v>
+        <v>-0.3596670273164657</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.3846386304601918</v>
+        <v>-0.375232968027443</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5330349069804005</v>
+        <v>0.4270913484275061</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4224260960009275</v>
+        <v>0.6085028859671858</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3930425803808136</v>
+        <v>0.2255854153401001</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4343019807177917</v>
+        <v>0.379357368435031</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4063797724265776</v>
-      </c>
+        <v>0.2418913238484973</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.01321640260353027</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.4085388932674926</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-0.07368234940306555</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-0.1070198579833858</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.1080750250941951</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.1183102115090504</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.05244954784002569</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.1212377602788528</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.1976122866906855</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.03447291215679107</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.001447980317488464</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.3088549070861667</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.2578297591592779</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.3768178938105072</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.8304875727968453</v>
+      </c>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -518,24 +650,75 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.04127197448859075</v>
+        <v>0.03293350680575683</v>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>0.06039239438758728</v>
+        <v>0.05080695341655181</v>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>0.06811070882203014</v>
+        <v>0.05741558435261409</v>
       </c>
       <c r="G3" t="n">
-        <v>0.06667570916281174</v>
+        <v>0.05898430135189713</v>
       </c>
       <c r="H3" t="n">
-        <v>0.06162636509034551</v>
+        <v>0.0565784181400702</v>
       </c>
       <c r="I3" t="n">
-        <v>0.06663628457132872</v>
+        <v>0.05868607878854772</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.05325089217110121</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.0607523167178206</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.05020743844196469</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.0699791456652953</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.07138789911816718</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.05085833899538811</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.07304348652495868</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.06768055290686406</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.06365817694538807</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.02139372384501209</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.08822528861906417</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.07156927949544066</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0.02456293908109812</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0.06221235494367305</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0.02793009420553279</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0.02977351400994221</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0.00659121318947396</v>
       </c>
     </row>
     <row r="4">
@@ -545,24 +728,75 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.3239446983594551</v>
+        <v>-0.3110561044774335</v>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>-0.2887931938914289</v>
+        <v>-0.2686380543701918</v>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>0.3610256939121302</v>
+        <v>0.008186721151914902</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.2168895792156875</v>
+        <v>-0.2171541409508627</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.2856188134319622</v>
+        <v>-0.2809909854521802</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.2199637365192384</v>
+        <v>-0.2126909321999807</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-0.1436532651969065</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-0.3083926291322202</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-0.2065356311511107</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-0.2143225879136349</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-0.07473352417654944</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-0.3369711151119406</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.005980885692627423</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-0.1546545370894981</v>
+      </c>
+      <c r="R4" t="n">
+        <v>-0.2372383629933376</v>
+      </c>
+      <c r="S4" t="n">
+        <v>-0.5023688090476083</v>
+      </c>
+      <c r="T4" t="n">
+        <v>-0.07805709403864657</v>
+      </c>
+      <c r="U4" t="n">
+        <v>-0.188528157885361</v>
+      </c>
+      <c r="V4" t="n">
+        <v>-0.2280981566358999</v>
+      </c>
+      <c r="W4" t="n">
+        <v>-0.3133645437642385</v>
+      </c>
+      <c r="X4" t="n">
+        <v>-0.3747883318544316</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0.03515302978284745</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0.02790623038655593</v>
       </c>
     </row>
     <row r="5">
@@ -572,24 +806,75 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.4274995037033422</v>
+        <v>0.4266445302534104</v>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>0.4624425617307449</v>
+        <v>0.4968936432688553</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>0.6573499217548775</v>
+        <v>0.7134579751517327</v>
       </c>
       <c r="G5" t="n">
-        <v>0.522766659159915</v>
+        <v>0.5451131820847904</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4375552247780745</v>
+        <v>0.4298224783827578</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5242039993623711</v>
+        <v>0.5508249818186541</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.5430298338349037</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.5684420723347245</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.5552699702664404</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.575325557482361</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.6414247215251878</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.4454647891165558</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.5677759508944532</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.6955889255581068</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.3959939513106306</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.5268767354228745</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.4446167454012109</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.5164587907816165</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.5524898540933959</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.6028662332977593</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0.7280375398390789</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0.06162415095642837</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.03065755333669287</v>
       </c>
     </row>
     <row r="6">
@@ -599,24 +884,75 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.2645089194606266</v>
+        <v>-0.2574997732991599</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>-0.1665744181425712</v>
+        <v>-0.168735271217353</v>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>-0.109496397071202</v>
+        <v>-0.0225218275507745</v>
       </c>
       <c r="G6" t="n">
-        <v>0.004934805980148974</v>
+        <v>-0.005211476239857595</v>
       </c>
       <c r="H6" t="n">
-        <v>0.02065491750250602</v>
+        <v>0.0002321959467225603</v>
       </c>
       <c r="I6" t="n">
-        <v>0.005148375946710792</v>
+        <v>-0.004161543132249423</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-0.04013875482345541</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.05612063358804344</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.1025990396612649</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-0.1545440408129345</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.1141301741369567</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-0.1266563859848372</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.1333320068314487</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.09399734443814031</v>
+      </c>
+      <c r="R6" t="n">
+        <v>-0.04672349304371198</v>
+      </c>
+      <c r="S6" t="n">
+        <v>-0.2629103742405735</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.1589434139821318</v>
+      </c>
+      <c r="U6" t="n">
+        <v>-0.1058177705464864</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.02649539909748065</v>
+      </c>
+      <c r="W6" t="n">
+        <v>-0.08776691653000711</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.07370602023262539</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0.009802392071497834</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0.007991275687465499</v>
       </c>
     </row>
     <row r="7">
@@ -627,23 +963,74 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
-        <v>0.6380077317838331</v>
+        <v>0.598822376247938</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6516879953356071</v>
+        <v>0.6107212392019017</v>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>0.8902330158887156</v>
+        <v>0.6923264694962541</v>
       </c>
       <c r="G7" t="n">
-        <v>0.6342829168255336</v>
+        <v>0.526983525452637</v>
       </c>
       <c r="H7" t="n">
-        <v>0.3360732152166998</v>
+        <v>0.2540421348169169</v>
       </c>
       <c r="I7" t="n">
-        <v>0.6024061392528383</v>
+        <v>0.5261667837525835</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.5813035557395559</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.4781238405944345</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.5945510059601166</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.2458696207859135</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.3664964308511479</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.562830792698728</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.4433469230677745</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.3671039396977405</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.5718291304287463</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.5768773684822843</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.6347340177253896</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.4596935501441321</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.5139472609757101</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.7586700256968802</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0.1589459477821145</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -654,23 +1041,74 @@
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
-        <v>0.3785739734363132</v>
+        <v>0.3329954594975929</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3676019924394046</v>
+        <v>0.3201042418881354</v>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>0.4248449015409902</v>
+        <v>0.3355042705795003</v>
       </c>
       <c r="G8" t="n">
-        <v>0.416592306931619</v>
+        <v>0.3478651971699352</v>
       </c>
       <c r="H8" t="n">
-        <v>0.4186265082299512</v>
+        <v>0.2969089382755387</v>
       </c>
       <c r="I8" t="n">
-        <v>0.4269591801703103</v>
+        <v>0.3558104086249295</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.345735192527769</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.365098572693223</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.2866711118336114</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.4616129281157406</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.5833458274818881</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.2423320533480413</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.7591711728603654</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.5288913227330373</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.3365859654893686</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.2252950938409177</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.4245864783970125</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.4110978643081494</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.1968231286184324</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.4261412483212504</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0.3128571403066884</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0.1050934713264846</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0.1196545089673275</v>
       </c>
     </row>
     <row r="9">
@@ -681,23 +1119,74 @@
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="n">
-        <v>0.3672899827862722</v>
+        <v>0.4426116002868843</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3588833797221106</v>
+        <v>0.4276491689400954</v>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>0.4584323759095543</v>
+        <v>0.5088576169055579</v>
       </c>
       <c r="G9" t="n">
-        <v>0.3960179904810393</v>
+        <v>0.4629750593293703</v>
       </c>
       <c r="H9" t="n">
-        <v>0.226858404593292</v>
+        <v>0.2877013904410228</v>
       </c>
       <c r="I9" t="n">
-        <v>0.4024299146834579</v>
+        <v>0.4782340584109332</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.4730404916037785</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.4809919493805861</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.428698362488374</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.5975622406107011</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.3552978037964453</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.4866854130595305</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.7077151548395086</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.2435168557685488</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.6665600428567309</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.4416313076904517</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.6340141150356756</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0.4237352499611113</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.4358603252413955</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0.4662091388969016</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0.4430864919859008</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>0.02335270549943606</v>
       </c>
     </row>
     <row r="10">
@@ -708,23 +1197,74 @@
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="n">
-        <v>0.7516136004269039</v>
+        <v>0.8173255593870614</v>
       </c>
       <c r="D10" t="n">
-        <v>0.7262095622816558</v>
+        <v>0.7935833906997333</v>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>0.5552937077382585</v>
+        <v>0.6311184971095474</v>
       </c>
       <c r="G10" t="n">
-        <v>0.8117737506908331</v>
+        <v>0.8851512138557585</v>
       </c>
       <c r="H10" t="n">
-        <v>0.6526446227321525</v>
+        <v>0.7489801259748162</v>
       </c>
       <c r="I10" t="n">
-        <v>0.7875413946242562</v>
+        <v>0.8806426648702045</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.9591376455855898</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.7565673170534246</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.8029357301925161</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.9674060520665121</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1.194363959722412</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.7542574925370261</v>
+      </c>
+      <c r="P10" t="n">
+        <v>1.428391237866615</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>1.074171421591972</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.6924359206415228</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.821053962974598</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.9507878499206778</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0.896213327006224</v>
+      </c>
+      <c r="V10" t="n">
+        <v>1.110200530818019</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.4676589145857515</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0.7037309854898374</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>0.05416279398180539</v>
       </c>
     </row>
     <row r="11">
@@ -735,23 +1275,74 @@
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="n">
-        <v>0.3798102094143315</v>
+        <v>0.4155777361832707</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4135597510995869</v>
+        <v>0.4478229501524228</v>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>0.4546096918375643</v>
+        <v>0.4416853231170753</v>
       </c>
       <c r="G11" t="n">
-        <v>0.4423868685793422</v>
+        <v>0.4520339945307955</v>
       </c>
       <c r="H11" t="n">
-        <v>0.3289318868567858</v>
+        <v>0.3791179485088395</v>
       </c>
       <c r="I11" t="n">
-        <v>0.4573079001943994</v>
+        <v>0.4714574905064179</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.4732883123519115</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.4681543362753872</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.4432813908004383</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.527185190504542</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.5233318101272673</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.4372092076241082</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.3778646321376163</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.6071000952856066</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.3937484082936381</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.5094003969301706</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.4402974904614564</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0.4653135923604281</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.5235779699052008</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0.4988571973100032</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0.3942542159141138</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0.05125546052898222</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0.08054928339848243</v>
       </c>
     </row>
     <row r="12">
@@ -762,23 +1353,74 @@
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="n">
-        <v>0.800661783689953</v>
+        <v>0.8274164598951924</v>
       </c>
       <c r="D12" t="n">
-        <v>0.7459484623446668</v>
+        <v>0.7482262423075713</v>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>0.8075730334259541</v>
+        <v>0.8012351065275636</v>
       </c>
       <c r="G12" t="n">
-        <v>0.8422053862182526</v>
+        <v>0.8015055490966779</v>
       </c>
       <c r="H12" t="n">
-        <v>0.6292326832255855</v>
+        <v>0.5851383517099206</v>
       </c>
       <c r="I12" t="n">
-        <v>0.779000211293549</v>
+        <v>0.7990126433683727</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.8656040578043848</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.6535496254898132</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.7201993812509127</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.8346019514089233</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1.054911032728778</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.7066414674511545</v>
+      </c>
+      <c r="P12" t="n">
+        <v>1.033091367816639</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>1.047538389615108</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.6863302552634823</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.753479007022942</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.582634696317514</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0.7982201206087071</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0.7896097368984462</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.8002877018737031</v>
+      </c>
+      <c r="X12" t="n">
+        <v>1.252023941239377</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -789,23 +1431,74 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.9869689190362195</v>
+        <v>0.9709645811247088</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9787515876914287</v>
+        <v>0.9666216940124102</v>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>0.8663853206802914</v>
+        <v>0.9125738705615186</v>
       </c>
       <c r="G13" t="n">
-        <v>0.9395372852379811</v>
+        <v>0.9135810504434609</v>
       </c>
       <c r="H13" t="n">
-        <v>0.8295547369241911</v>
+        <v>0.8247819182367573</v>
       </c>
       <c r="I13" t="n">
-        <v>0.9224465794657603</v>
+        <v>0.9118441812639587</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.8905440093178907</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.9259971349595172</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.8449990637162367</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1.174770514337292</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.9930751123261828</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.8787227902151529</v>
+      </c>
+      <c r="P13" t="n">
+        <v>1.000564509482604</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.9999823640916958</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.9442037340355313</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.9118449333764453</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.8795473135606559</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0.9776788106187327</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0.9491070146891983</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0.6604916116421576</v>
+      </c>
+      <c r="X13" t="n">
+        <v>1.032001527079374</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0.0850614213616574</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0.1266279897932048</v>
       </c>
     </row>
     <row r="14">
@@ -816,23 +1509,74 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>0.1369406995516451</v>
+        <v>0.1718466589537598</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1451926888667908</v>
+        <v>0.1841484508893274</v>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>0.2938400424543438</v>
+        <v>0.3862058249628295</v>
       </c>
       <c r="G14" t="n">
-        <v>0.15210688467165</v>
+        <v>0.1999313565492728</v>
       </c>
       <c r="H14" t="n">
-        <v>0.01387517896209382</v>
+        <v>0.07916889748960407</v>
       </c>
       <c r="I14" t="n">
-        <v>0.1429599702562385</v>
+        <v>0.1903094031949638</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.21302000763473</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.1369416966534953</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.155538722922047</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.2452023594798356</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.2361662000101486</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.1412462940157818</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.3248275508723477</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.1876486187906158</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.1870123005209375</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.08802066460591836</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.3389894076310619</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0.06315743903434785</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0.3752252876465313</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0.09587690443449781</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0.06324089059490771</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0.005586905496662999</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>0.02087529828937386</v>
       </c>
     </row>
     <row r="15">
@@ -845,19 +1589,66 @@
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
-        <v>-1.1160557292987</v>
+        <v>-1.050829179728364</v>
       </c>
       <c r="F15" t="n">
-        <v>-1.058197728942757</v>
+        <v>-1.040200962062119</v>
       </c>
       <c r="G15" t="n">
-        <v>-1.009006548228627</v>
+        <v>-1.004322752213272</v>
       </c>
       <c r="H15" t="n">
-        <v>-1.18237943677006</v>
+        <v>-1.149602845109496</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.9968217194060317</v>
+        <v>-0.9984706524474731</v>
+      </c>
+      <c r="J15" t="n">
+        <v>-1.052021139067762</v>
+      </c>
+      <c r="K15" t="n">
+        <v>-0.9294893642298976</v>
+      </c>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="n">
+        <v>-1.136666190465586</v>
+      </c>
+      <c r="O15" t="n">
+        <v>-0.8946888949404204</v>
+      </c>
+      <c r="P15" t="n">
+        <v>-1.15449154782546</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>-1.114482816530129</v>
+      </c>
+      <c r="R15" t="n">
+        <v>-0.9374556603833734</v>
+      </c>
+      <c r="S15" t="n">
+        <v>-0.8432154741475543</v>
+      </c>
+      <c r="T15" t="n">
+        <v>-1.114551416138676</v>
+      </c>
+      <c r="U15" t="n">
+        <v>-0.9352464100822732</v>
+      </c>
+      <c r="V15" t="n">
+        <v>-0.9510298563021748</v>
+      </c>
+      <c r="W15" t="n">
+        <v>-0.8632049682420729</v>
+      </c>
+      <c r="X15" t="n">
+        <v>-1.243392049422181</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>0.5160921064929431</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>0.3892714750898331</v>
       </c>
     </row>
     <row r="16">
@@ -870,19 +1661,70 @@
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
-        <v>-0.3863116468119924</v>
+        <v>-0.3908151934010236</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.3547248506549109</v>
+        <v>-0.337151351998511</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.3720469291924142</v>
+        <v>-0.3613113690209812</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.3740857804406019</v>
+        <v>-0.3796714867221856</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.370935762316822</v>
+        <v>-0.3629806153200745</v>
+      </c>
+      <c r="J16" t="n">
+        <v>-0.3927795944920378</v>
+      </c>
+      <c r="K16" t="n">
+        <v>-0.2833588079350921</v>
+      </c>
+      <c r="L16" t="n">
+        <v>-0.2327549160526793</v>
+      </c>
+      <c r="M16" t="n">
+        <v>-0.6074204513995106</v>
+      </c>
+      <c r="N16" t="n">
+        <v>-0.3532981080049933</v>
+      </c>
+      <c r="O16" t="n">
+        <v>-0.3862563340245289</v>
+      </c>
+      <c r="P16" t="n">
+        <v>-0.315700987833142</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>-0.3628749633667071</v>
+      </c>
+      <c r="R16" t="n">
+        <v>-0.5570116958537704</v>
+      </c>
+      <c r="S16" t="n">
+        <v>-0.2252495425645419</v>
+      </c>
+      <c r="T16" t="n">
+        <v>-0.3709084832213077</v>
+      </c>
+      <c r="U16" t="n">
+        <v>-0.3750894081737554</v>
+      </c>
+      <c r="V16" t="n">
+        <v>-0.3889318656480695</v>
+      </c>
+      <c r="W16" t="n">
+        <v>-0.307672998866131</v>
+      </c>
+      <c r="X16" t="n">
+        <v>-0.3067768362899017</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0.05441562878594887</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>0.06655234352006274</v>
       </c>
     </row>
     <row r="17">
@@ -895,19 +1737,70 @@
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
-        <v>-0.118837232128166</v>
+        <v>-0.03994026348645136</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.02316977472289983</v>
+        <v>-0.04349538286778701</v>
       </c>
       <c r="G17" t="n">
-        <v>0.02404113552624051</v>
+        <v>0.02157111482613456</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.008879692833420657</v>
+        <v>0.0128336369611939</v>
       </c>
       <c r="I17" t="n">
-        <v>0.02431671123022212</v>
+        <v>0.01938159981063712</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.06022193622994988</v>
+      </c>
+      <c r="K17" t="n">
+        <v>-0.003297727268798967</v>
+      </c>
+      <c r="L17" t="n">
+        <v>-0.00850585120351322</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.07724880429073201</v>
+      </c>
+      <c r="N17" t="n">
+        <v>-0.006003816102489646</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.05560758950875244</v>
+      </c>
+      <c r="P17" t="n">
+        <v>-0.03121617460888204</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.03047162405807931</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.07724891070312004</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.02008959530074963</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.1023885954475065</v>
+      </c>
+      <c r="U17" t="n">
+        <v>-0.002988405361712019</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0.006142358535025567</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0.06395673432075015</v>
+      </c>
+      <c r="X17" t="n">
+        <v>-0.0830607826921818</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>0.004805993195136018</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>0.006243335830654275</v>
       </c>
     </row>
     <row r="18">
@@ -920,173 +1813,466 @@
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
-        <v>0.08147401714881683</v>
+        <v>0.1159624805032701</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.1864649958320523</v>
+        <v>-0.1645238296751658</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.07392110706209443</v>
+        <v>-0.05600024055658809</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.06137186431921215</v>
+        <v>-0.03455394962497098</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.07526985138159009</v>
+        <v>-0.06142905522380834</v>
+      </c>
+      <c r="J18" t="n">
+        <v>-0.00342479746260841</v>
+      </c>
+      <c r="K18" t="n">
+        <v>-0.1440680191224907</v>
+      </c>
+      <c r="L18" t="n">
+        <v>-0.06326063965410909</v>
+      </c>
+      <c r="M18" t="n">
+        <v>-0.02678838740180837</v>
+      </c>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="n">
+        <v>-0.04568068250007021</v>
+      </c>
+      <c r="U18" t="n">
+        <v>-0.07085536826493438</v>
+      </c>
+      <c r="V18" t="n">
+        <v>-0.01427655965971534</v>
+      </c>
+      <c r="W18" t="n">
+        <v>-0.06777713987208746</v>
+      </c>
+      <c r="X18" t="n">
+        <v>-0.1296990657686618</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>0.01197559944487173</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>0.006319193147230384</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>cor_branca</t>
+          <t>class_renda</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
-        <v>0.08280307809609172</v>
+        <v>-0.2881790248885415</v>
       </c>
       <c r="F19" t="n">
-        <v>0.1195184858215987</v>
+        <v>-0.2339076319790845</v>
       </c>
       <c r="G19" t="n">
-        <v>0.102203065914221</v>
+        <v>-0.2159044989116853</v>
       </c>
       <c r="H19" t="n">
-        <v>0.2944222657940227</v>
+        <v>-0.2433643249848889</v>
       </c>
       <c r="I19" t="n">
-        <v>0.1076178163220726</v>
+        <v>-0.2178226482079839</v>
+      </c>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="n">
+        <v>-0.2933804799586436</v>
+      </c>
+      <c r="M19" t="n">
+        <v>-0.1509994338043972</v>
+      </c>
+      <c r="N19" t="n">
+        <v>-0.08090520776461688</v>
+      </c>
+      <c r="O19" t="n">
+        <v>-0.3599425184771486</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.04100724562746618</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>-0.186057490840102</v>
+      </c>
+      <c r="R19" t="n">
+        <v>-0.3721940162516757</v>
+      </c>
+      <c r="S19" t="n">
+        <v>-0.2937424184787101</v>
+      </c>
+      <c r="T19" t="n">
+        <v>-0.3623125631581927</v>
+      </c>
+      <c r="U19" t="n">
+        <v>-0.04783038232018201</v>
+      </c>
+      <c r="V19" t="n">
+        <v>-0.2624848801297247</v>
+      </c>
+      <c r="W19" t="n">
+        <v>-0.41573486882464</v>
+      </c>
+      <c r="X19" t="n">
+        <v>-0.1523942277619023</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>0.02325003385014245</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>0.02531099431058551</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>cor_preta</t>
+          <t>r_norte</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="n">
-        <v>0.2087987937623225</v>
+        <v>-0.08060485451772936</v>
       </c>
       <c r="F20" t="n">
-        <v>0.1365495272421828</v>
+        <v>0.01508341421044419</v>
       </c>
       <c r="G20" t="n">
-        <v>0.1408972207911487</v>
+        <v>-0.07864926074281797</v>
       </c>
       <c r="H20" t="n">
-        <v>0.2441510644712671</v>
+        <v>-0.04664333649020832</v>
       </c>
       <c r="I20" t="n">
-        <v>0.146994407059571</v>
+        <v>-0.07133994702509107</v>
+      </c>
+      <c r="J20" t="n">
+        <v>-0.1276130460618353</v>
+      </c>
+      <c r="K20" t="n">
+        <v>-0.0676101683926118</v>
+      </c>
+      <c r="L20" t="n">
+        <v>-0.1026926659344388</v>
+      </c>
+      <c r="M20" t="n">
+        <v>-0.1824204452457752</v>
+      </c>
+      <c r="N20" t="n">
+        <v>-0.04297441018177948</v>
+      </c>
+      <c r="O20" t="n">
+        <v>-0.1526772012090504</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.02599433906575027</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>-0.1206258431499396</v>
+      </c>
+      <c r="R20" t="n">
+        <v>-0.223680107221946</v>
+      </c>
+      <c r="S20" t="n">
+        <v>-0.07233791517940329</v>
+      </c>
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" t="inlineStr"/>
+      <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
+      <c r="X20" t="inlineStr"/>
+      <c r="Y20" t="n">
+        <v>0.003798336613726669</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>0.003417064095384525</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>cor_amarela</t>
+          <t>r_nordeste</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>-0.09527276205592133</v>
+        <v>0.0921217511244581</v>
       </c>
       <c r="F21" t="n">
-        <v>0.202516984368705</v>
+        <v>0.09505130207862908</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.05124194909719267</v>
+        <v>0.09453158360246315</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.2626580699449537</v>
+        <v>0.162725798425864</v>
       </c>
       <c r="I21" t="n">
-        <v>-0.04692902847923715</v>
+        <v>0.09860595781126287</v>
+      </c>
+      <c r="J21" t="n">
+        <v>-0.01460456455368297</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.2599357637618283</v>
+      </c>
+      <c r="L21" t="n">
+        <v>-0.004188334205599924</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.1040124665767261</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.1171087526688932</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.03440991604363898</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.1240904671315738</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0.107715875993416</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0.04676129231926173</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0.02468320080010153</v>
+      </c>
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr"/>
+      <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
+      <c r="X21" t="inlineStr"/>
+      <c r="Y21" t="n">
+        <v>0.002311956082728097</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>0.001506210284155824</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>cor_parda</t>
+          <t>r_sudeste</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
-        <v>0.1352264483289186</v>
+        <v>0.1699172765767713</v>
       </c>
       <c r="F22" t="n">
-        <v>0.139631273505433</v>
+        <v>0.02028045345909574</v>
       </c>
       <c r="G22" t="n">
-        <v>0.09030297455534733</v>
+        <v>0.0911198878432114</v>
       </c>
       <c r="H22" t="n">
-        <v>0.312740016891105</v>
+        <v>0.1464405133239115</v>
       </c>
       <c r="I22" t="n">
-        <v>0.09700886924869703</v>
+        <v>0.0931895263726438</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.0364237020270942</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.1218026219699975</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.01646739137558623</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.0504984675164259</v>
+      </c>
+      <c r="N22" t="n">
+        <v>-0.03473327890864224</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0.1528626977925132</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.05399304299764739</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>-0.1018380319131177</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0.112945054888285</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0.2111215094373347</v>
+      </c>
+      <c r="T22" t="inlineStr"/>
+      <c r="U22" t="inlineStr"/>
+      <c r="V22" t="inlineStr"/>
+      <c r="W22" t="inlineStr"/>
+      <c r="X22" t="inlineStr"/>
+      <c r="Y22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>0.0008252733553956642</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>cor_indigena</t>
+          <t>r_sul</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
-        <v>0.18555559844252</v>
+        <v>0.09882274831369456</v>
       </c>
       <c r="F23" t="n">
-        <v>-0.2371905770257908</v>
+        <v>-0.05855810603329039</v>
       </c>
       <c r="G23" t="n">
-        <v>0.09959842776084385</v>
+        <v>0.006041644640203639</v>
       </c>
       <c r="H23" t="n">
-        <v>-0.1662203233685123</v>
+        <v>0.0003815201101424374</v>
       </c>
       <c r="I23" t="n">
-        <v>0.1016877082745947</v>
+        <v>0.009663544903424833</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.05436641184662697</v>
+      </c>
+      <c r="K23" t="n">
+        <v>-0.03277356942050424</v>
+      </c>
+      <c r="L23" t="n">
+        <v>-0.09433784348177857</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.005244274603719849</v>
+      </c>
+      <c r="N23" t="n">
+        <v>-0.05339171751945629</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0.01088759598463186</v>
+      </c>
+      <c r="P23" t="n">
+        <v>-0.1906049666577723</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0.04352497960318333</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0.09293703197646938</v>
+      </c>
+      <c r="S23" t="n">
+        <v>-0.06446049511021867</v>
+      </c>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
+      <c r="X23" t="inlineStr"/>
+      <c r="Y23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>0.001073550074042892</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>activity_class</t>
+          <t>r_centro_oeste</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
+      <c r="E24" t="n">
+        <v>0.145164401028334</v>
+      </c>
       <c r="F24" t="n">
-        <v>-0.005280759954039123</v>
+        <v>-0.06367034256277451</v>
       </c>
       <c r="G24" t="n">
-        <v>0.04352925724808123</v>
+        <v>0.1070567569106278</v>
       </c>
       <c r="H24" t="n">
-        <v>-0.2179209505540413</v>
+        <v>0.1097171415471539</v>
       </c>
       <c r="I24" t="n">
-        <v>0.009703778000036856</v>
+        <v>0.111772241781431</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.06464389934048996</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.1271842453517322</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.1110691028454016</v>
+      </c>
+      <c r="M24" t="n">
+        <v>-0.08435462144129985</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.1220656790232404</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0.07282720289428674</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0.03897666531430082</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.1924607797424207</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0.1686490147274442</v>
+      </c>
+      <c r="S24" t="n">
+        <v>-0.06453338779199531</v>
+      </c>
+      <c r="T24" t="inlineStr"/>
+      <c r="U24" t="inlineStr"/>
+      <c r="V24" t="inlineStr"/>
+      <c r="W24" t="inlineStr"/>
+      <c r="X24" t="inlineStr"/>
+      <c r="Y24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>0.0003850080871679181</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>renda_pc</t>
+          <t>activity_class</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -1094,16 +2280,67 @@
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="n">
-        <v>-0.09493710291915854</v>
+        <v>-0.04594539837098988</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.08878493409234628</v>
+        <v>-0.01194932124140764</v>
       </c>
       <c r="H25" t="n">
-        <v>-0.07884469234021553</v>
+        <v>-0.2503771689580481</v>
       </c>
       <c r="I25" t="n">
-        <v>-0.09025491332407781</v>
+        <v>-0.0387610401203585</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.01591386380226879</v>
+      </c>
+      <c r="K25" t="n">
+        <v>-0.09923171397193659</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.05521228839112366</v>
+      </c>
+      <c r="M25" t="n">
+        <v>-0.2295472150152053</v>
+      </c>
+      <c r="N25" t="n">
+        <v>-0.04873927902365896</v>
+      </c>
+      <c r="O25" t="n">
+        <v>-0.04021950652565973</v>
+      </c>
+      <c r="P25" t="n">
+        <v>-0.05272265918509387</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>-0.04648203534646526</v>
+      </c>
+      <c r="R25" t="n">
+        <v>-0.04718315574884838</v>
+      </c>
+      <c r="S25" t="n">
+        <v>-0.03768658348680035</v>
+      </c>
+      <c r="T25" t="n">
+        <v>-0.1275140668007314</v>
+      </c>
+      <c r="U25" t="n">
+        <v>-0.04075708757652695</v>
+      </c>
+      <c r="V25" t="n">
+        <v>-0.05339634034079128</v>
+      </c>
+      <c r="W25" t="n">
+        <v>-0.03052088131689951</v>
+      </c>
+      <c r="X25" t="n">
+        <v>0.05681146782512388</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>0.0007266996756689666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>